<commit_message>
Update works images 2026-01-18 06:32:51
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A486"/>
+  <dimension ref="A1:A485"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -452,3400 +452,3393 @@
     <row r="1">
       <c r="A1" s="0" t="inlineStr">
         <is>
-          <t>r6qvrdxz</t>
+          <t>8a24swce</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>8a24swce</t>
+          <t>0xl7t7xl</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>0xl7t7xl</t>
+          <t>hlzcq1o6</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>hlzcq1o6</t>
+          <t>7yknd8pc</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>7yknd8pc</t>
+          <t>hty8ut3e</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>hty8ut3e</t>
+          <t>up73h59u</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>up73h59u</t>
+          <t>949vogeu</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>949vogeu</t>
+          <t>ghlktp23</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>ghlktp23</t>
+          <t>ofh3kwsi</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>ofh3kwsi</t>
+          <t>ggu21lkq</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>ggu21lkq</t>
+          <t>j0writd2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>j0writd2</t>
+          <t>vcjhum2r</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>vcjhum2r</t>
+          <t>fuxp1un3</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>fuxp1un3</t>
+          <t>dmy3qb36</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>dmy3qb36</t>
+          <t>3cs680lw</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>3cs680lw</t>
+          <t>3l5ikk8t</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>3l5ikk8t</t>
+          <t>8fcbyk1m</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>8fcbyk1m</t>
+          <t>y1puz53f</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>y1puz53f</t>
+          <t>f7m05b4u</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>f7m05b4u</t>
+          <t>axri1ag2</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>axri1ag2</t>
+          <t>n6s5h4v9</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>n6s5h4v9</t>
+          <t>lpv0bvsw</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>lpv0bvsw</t>
+          <t>p2ysb4km</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>p2ysb4km</t>
+          <t>0rh82tbc</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>r88cbjqo</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="474">
       <c r="A474" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="475">
       <c r="A475" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="476">
       <c r="A476" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="477">
       <c r="A477" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="478">
       <c r="A478" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="479">
       <c r="A479" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="480">
       <c r="A480" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="481">
       <c r="A481" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="482">
       <c r="A482" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="483">
       <c r="A483" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="484">
       <c r="A484" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="485">
       <c r="A485" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="486">
-      <c r="A486" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3862,7 +3855,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4075,19 +4068,36 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="0" t="inlineStr">
         <is>
           <t>0vy0bibt</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月18日 05_40_10.png</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="0" t="inlineStr">
         <is>
           <t>2026-01-18 05:43:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>r6qvrdxz</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月18日 06_29_52.png</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2026-01-18 06:32:41</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-18 07:01:36
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A485"/>
+  <dimension ref="A1:A484"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -452,3393 +452,3386 @@
     <row r="1">
       <c r="A1" s="0" t="inlineStr">
         <is>
-          <t>8a24swce</t>
+          <t>0xl7t7xl</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>0xl7t7xl</t>
+          <t>hlzcq1o6</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>hlzcq1o6</t>
+          <t>7yknd8pc</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>7yknd8pc</t>
+          <t>hty8ut3e</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>hty8ut3e</t>
+          <t>up73h59u</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>up73h59u</t>
+          <t>949vogeu</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>949vogeu</t>
+          <t>ghlktp23</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>ghlktp23</t>
+          <t>ofh3kwsi</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>ofh3kwsi</t>
+          <t>ggu21lkq</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>ggu21lkq</t>
+          <t>j0writd2</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>j0writd2</t>
+          <t>vcjhum2r</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>vcjhum2r</t>
+          <t>fuxp1un3</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>fuxp1un3</t>
+          <t>dmy3qb36</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>dmy3qb36</t>
+          <t>3cs680lw</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>3cs680lw</t>
+          <t>3l5ikk8t</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>3l5ikk8t</t>
+          <t>8fcbyk1m</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>8fcbyk1m</t>
+          <t>y1puz53f</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>y1puz53f</t>
+          <t>f7m05b4u</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>f7m05b4u</t>
+          <t>axri1ag2</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>axri1ag2</t>
+          <t>n6s5h4v9</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>n6s5h4v9</t>
+          <t>lpv0bvsw</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>lpv0bvsw</t>
+          <t>p2ysb4km</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>p2ysb4km</t>
+          <t>0rh82tbc</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>r88cbjqo</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="474">
       <c r="A474" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="475">
       <c r="A475" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="476">
       <c r="A476" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="477">
       <c r="A477" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="478">
       <c r="A478" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="479">
       <c r="A479" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="480">
       <c r="A480" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="481">
       <c r="A481" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="482">
       <c r="A482" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="483">
       <c r="A483" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="484">
       <c r="A484" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="485">
-      <c r="A485" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3855,7 +3848,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4085,19 +4078,36 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="0" t="inlineStr">
         <is>
           <t>r6qvrdxz</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月18日 06_29_52.png</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="0" t="inlineStr">
         <is>
           <t>2026-01-18 06:32:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>8a24swce</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月18日 07_00_29.png</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2026-01-18 07:01:32</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-18 07:09:51
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A484"/>
+  <dimension ref="A1:A483"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -452,3386 +452,3379 @@
     <row r="1">
       <c r="A1" s="0" t="inlineStr">
         <is>
-          <t>0xl7t7xl</t>
+          <t>hlzcq1o6</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>hlzcq1o6</t>
+          <t>7yknd8pc</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>7yknd8pc</t>
+          <t>hty8ut3e</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>hty8ut3e</t>
+          <t>up73h59u</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>up73h59u</t>
+          <t>949vogeu</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>949vogeu</t>
+          <t>ghlktp23</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>ghlktp23</t>
+          <t>ofh3kwsi</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>ofh3kwsi</t>
+          <t>ggu21lkq</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>ggu21lkq</t>
+          <t>j0writd2</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>j0writd2</t>
+          <t>vcjhum2r</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>vcjhum2r</t>
+          <t>fuxp1un3</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>fuxp1un3</t>
+          <t>dmy3qb36</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>dmy3qb36</t>
+          <t>3cs680lw</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>3cs680lw</t>
+          <t>3l5ikk8t</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>3l5ikk8t</t>
+          <t>8fcbyk1m</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>8fcbyk1m</t>
+          <t>y1puz53f</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>y1puz53f</t>
+          <t>f7m05b4u</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>f7m05b4u</t>
+          <t>axri1ag2</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>axri1ag2</t>
+          <t>n6s5h4v9</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>n6s5h4v9</t>
+          <t>lpv0bvsw</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>lpv0bvsw</t>
+          <t>p2ysb4km</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>p2ysb4km</t>
+          <t>0rh82tbc</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>r88cbjqo</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="474">
       <c r="A474" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="475">
       <c r="A475" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="476">
       <c r="A476" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="477">
       <c r="A477" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="478">
       <c r="A478" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="479">
       <c r="A479" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="480">
       <c r="A480" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="481">
       <c r="A481" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="482">
       <c r="A482" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="483">
       <c r="A483" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="484">
-      <c r="A484" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3848,7 +3841,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4095,19 +4088,36 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="0" t="inlineStr">
         <is>
           <t>8a24swce</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月18日 07_00_29.png</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="0" t="inlineStr">
         <is>
           <t>2026-01-18 07:01:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>0xl7t7xl</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月18日 07_08_24.png</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2026-01-18 07:09:47</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-18 07:39:12
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A483"/>
+  <dimension ref="A1:A482"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -452,3379 +452,3372 @@
     <row r="1">
       <c r="A1" s="0" t="inlineStr">
         <is>
-          <t>hlzcq1o6</t>
+          <t>7yknd8pc</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>7yknd8pc</t>
+          <t>hty8ut3e</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>hty8ut3e</t>
+          <t>up73h59u</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>up73h59u</t>
+          <t>949vogeu</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>949vogeu</t>
+          <t>ghlktp23</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>ghlktp23</t>
+          <t>ofh3kwsi</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>ofh3kwsi</t>
+          <t>ggu21lkq</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>ggu21lkq</t>
+          <t>j0writd2</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>j0writd2</t>
+          <t>vcjhum2r</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>vcjhum2r</t>
+          <t>fuxp1un3</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>fuxp1un3</t>
+          <t>dmy3qb36</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>dmy3qb36</t>
+          <t>3cs680lw</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>3cs680lw</t>
+          <t>3l5ikk8t</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>3l5ikk8t</t>
+          <t>8fcbyk1m</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>8fcbyk1m</t>
+          <t>y1puz53f</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>y1puz53f</t>
+          <t>f7m05b4u</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>f7m05b4u</t>
+          <t>axri1ag2</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>axri1ag2</t>
+          <t>n6s5h4v9</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>n6s5h4v9</t>
+          <t>lpv0bvsw</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>lpv0bvsw</t>
+          <t>p2ysb4km</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>p2ysb4km</t>
+          <t>0rh82tbc</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>r88cbjqo</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="474">
       <c r="A474" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="475">
       <c r="A475" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="476">
       <c r="A476" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="477">
       <c r="A477" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="478">
       <c r="A478" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="479">
       <c r="A479" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="480">
       <c r="A480" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="481">
       <c r="A481" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="482">
       <c r="A482" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="483">
-      <c r="A483" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3841,7 +3834,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4105,19 +4098,36 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="0" t="inlineStr">
         <is>
           <t>0xl7t7xl</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月18日 07_08_24.png</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="0" t="inlineStr">
         <is>
           <t>2026-01-18 07:09:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>hlzcq1o6</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月18日 07_37_14.png</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2026-01-18 07:39:08</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-18 08:51:42
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A482"/>
+  <dimension ref="A1:A481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -452,3372 +452,3365 @@
     <row r="1">
       <c r="A1" s="0" t="inlineStr">
         <is>
-          <t>7yknd8pc</t>
+          <t>hty8ut3e</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>hty8ut3e</t>
+          <t>up73h59u</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>up73h59u</t>
+          <t>949vogeu</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>949vogeu</t>
+          <t>ghlktp23</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>ghlktp23</t>
+          <t>ofh3kwsi</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>ofh3kwsi</t>
+          <t>ggu21lkq</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>ggu21lkq</t>
+          <t>j0writd2</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>j0writd2</t>
+          <t>vcjhum2r</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>vcjhum2r</t>
+          <t>fuxp1un3</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>fuxp1un3</t>
+          <t>dmy3qb36</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>dmy3qb36</t>
+          <t>3cs680lw</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>3cs680lw</t>
+          <t>3l5ikk8t</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>3l5ikk8t</t>
+          <t>8fcbyk1m</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>8fcbyk1m</t>
+          <t>y1puz53f</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>y1puz53f</t>
+          <t>f7m05b4u</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>f7m05b4u</t>
+          <t>axri1ag2</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>axri1ag2</t>
+          <t>n6s5h4v9</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>n6s5h4v9</t>
+          <t>lpv0bvsw</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>lpv0bvsw</t>
+          <t>p2ysb4km</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>p2ysb4km</t>
+          <t>0rh82tbc</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>r88cbjqo</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="474">
       <c r="A474" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="475">
       <c r="A475" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="476">
       <c r="A476" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="477">
       <c r="A477" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="478">
       <c r="A478" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="479">
       <c r="A479" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="480">
       <c r="A480" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="481">
       <c r="A481" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="482">
-      <c r="A482" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3834,7 +3827,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4115,19 +4108,36 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="0" t="inlineStr">
         <is>
           <t>hlzcq1o6</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月18日 07_37_14.png</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" s="0" t="inlineStr">
         <is>
           <t>2026-01-18 07:39:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>7yknd8pc</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月18日 08_44_52.png</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2026-01-18 08:51:37</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-18 09:59:53
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A481"/>
+  <dimension ref="A1:A480"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -452,3365 +452,3358 @@
     <row r="1">
       <c r="A1" s="0" t="inlineStr">
         <is>
-          <t>hty8ut3e</t>
+          <t>up73h59u</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>up73h59u</t>
+          <t>949vogeu</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>949vogeu</t>
+          <t>ghlktp23</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>ghlktp23</t>
+          <t>ofh3kwsi</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>ofh3kwsi</t>
+          <t>ggu21lkq</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>ggu21lkq</t>
+          <t>j0writd2</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>j0writd2</t>
+          <t>vcjhum2r</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>vcjhum2r</t>
+          <t>fuxp1un3</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>fuxp1un3</t>
+          <t>dmy3qb36</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>dmy3qb36</t>
+          <t>3cs680lw</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>3cs680lw</t>
+          <t>3l5ikk8t</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>3l5ikk8t</t>
+          <t>8fcbyk1m</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>8fcbyk1m</t>
+          <t>y1puz53f</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>y1puz53f</t>
+          <t>f7m05b4u</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>f7m05b4u</t>
+          <t>axri1ag2</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>axri1ag2</t>
+          <t>n6s5h4v9</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>n6s5h4v9</t>
+          <t>lpv0bvsw</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>lpv0bvsw</t>
+          <t>p2ysb4km</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>p2ysb4km</t>
+          <t>0rh82tbc</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>r88cbjqo</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="474">
       <c r="A474" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="475">
       <c r="A475" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="476">
       <c r="A476" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="477">
       <c r="A477" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="478">
       <c r="A478" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="479">
       <c r="A479" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="480">
       <c r="A480" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="481">
-      <c r="A481" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3827,7 +3820,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4125,19 +4118,36 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="0" t="inlineStr">
         <is>
           <t>7yknd8pc</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月18日 08_44_52.png</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="0" t="inlineStr">
         <is>
           <t>2026-01-18 08:51:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>hty8ut3e</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月18日 09_58_09.png</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2026-01-18 09:59:49</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-18 10:35:18
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A480"/>
+  <dimension ref="A1:A479"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -452,3358 +452,3351 @@
     <row r="1">
       <c r="A1" s="0" t="inlineStr">
         <is>
-          <t>up73h59u</t>
+          <t>949vogeu</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>949vogeu</t>
+          <t>ghlktp23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>ghlktp23</t>
+          <t>ofh3kwsi</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>ofh3kwsi</t>
+          <t>ggu21lkq</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>ggu21lkq</t>
+          <t>j0writd2</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>j0writd2</t>
+          <t>vcjhum2r</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>vcjhum2r</t>
+          <t>fuxp1un3</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>fuxp1un3</t>
+          <t>dmy3qb36</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>dmy3qb36</t>
+          <t>3cs680lw</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>3cs680lw</t>
+          <t>3l5ikk8t</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>3l5ikk8t</t>
+          <t>8fcbyk1m</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>8fcbyk1m</t>
+          <t>y1puz53f</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>y1puz53f</t>
+          <t>f7m05b4u</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>f7m05b4u</t>
+          <t>axri1ag2</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>axri1ag2</t>
+          <t>n6s5h4v9</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>n6s5h4v9</t>
+          <t>lpv0bvsw</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>lpv0bvsw</t>
+          <t>p2ysb4km</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>p2ysb4km</t>
+          <t>0rh82tbc</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>r88cbjqo</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="474">
       <c r="A474" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="475">
       <c r="A475" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="476">
       <c r="A476" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="477">
       <c r="A477" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="478">
       <c r="A478" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="479">
       <c r="A479" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="480">
-      <c r="A480" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3820,7 +3813,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4135,19 +4128,36 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="0" t="inlineStr">
         <is>
           <t>hty8ut3e</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月18日 09_58_09.png</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" s="0" t="inlineStr">
         <is>
           <t>2026-01-18 09:59:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>up73h59u</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月18日 10_33_10.png</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2026-01-18 10:35:13</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-18 11:40:10
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A479"/>
+  <dimension ref="A1:A478"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -452,3351 +452,3344 @@
     <row r="1">
       <c r="A1" s="0" t="inlineStr">
         <is>
-          <t>949vogeu</t>
+          <t>ghlktp23</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>ghlktp23</t>
+          <t>ofh3kwsi</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>ofh3kwsi</t>
+          <t>ggu21lkq</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>ggu21lkq</t>
+          <t>j0writd2</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>j0writd2</t>
+          <t>vcjhum2r</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>vcjhum2r</t>
+          <t>fuxp1un3</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>fuxp1un3</t>
+          <t>dmy3qb36</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>dmy3qb36</t>
+          <t>3cs680lw</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>3cs680lw</t>
+          <t>3l5ikk8t</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>3l5ikk8t</t>
+          <t>8fcbyk1m</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>8fcbyk1m</t>
+          <t>y1puz53f</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>y1puz53f</t>
+          <t>f7m05b4u</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>f7m05b4u</t>
+          <t>axri1ag2</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>axri1ag2</t>
+          <t>n6s5h4v9</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>n6s5h4v9</t>
+          <t>lpv0bvsw</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>lpv0bvsw</t>
+          <t>p2ysb4km</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>p2ysb4km</t>
+          <t>0rh82tbc</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>r88cbjqo</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="474">
       <c r="A474" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="475">
       <c r="A475" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="476">
       <c r="A476" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="477">
       <c r="A477" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="478">
       <c r="A478" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="479">
-      <c r="A479" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3813,7 +3806,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4145,19 +4138,36 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="0" t="inlineStr">
         <is>
           <t>up73h59u</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月18日 10_33_10.png</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" s="0" t="inlineStr">
         <is>
           <t>2026-01-18 10:35:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>949vogeu</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月18日 11_38_38.png</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2026-01-18 11:40:05</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-20 15:40:40
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A478"/>
+  <dimension ref="A1:A476"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -452,3344 +452,3330 @@
     <row r="1">
       <c r="A1" s="0" t="inlineStr">
         <is>
-          <t>ghlktp23</t>
+          <t>ofh3kwsi</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>ofh3kwsi</t>
+          <t>j0writd2</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>ggu21lkq</t>
+          <t>vcjhum2r</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>j0writd2</t>
+          <t>fuxp1un3</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>vcjhum2r</t>
+          <t>dmy3qb36</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>fuxp1un3</t>
+          <t>3cs680lw</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>dmy3qb36</t>
+          <t>3l5ikk8t</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>3cs680lw</t>
+          <t>8fcbyk1m</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>3l5ikk8t</t>
+          <t>y1puz53f</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>8fcbyk1m</t>
+          <t>f7m05b4u</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>y1puz53f</t>
+          <t>axri1ag2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>f7m05b4u</t>
+          <t>n6s5h4v9</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>axri1ag2</t>
+          <t>lpv0bvsw</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>n6s5h4v9</t>
+          <t>p2ysb4km</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>lpv0bvsw</t>
+          <t>0rh82tbc</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>p2ysb4km</t>
+          <t>r88cbjqo</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="474">
       <c r="A474" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="475">
       <c r="A475" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="476">
       <c r="A476" s="0" t="inlineStr">
-        <is>
-          <t>c47md6bk</t>
-        </is>
-      </c>
-    </row>
-    <row r="477">
-      <c r="A477" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="478">
-      <c r="A478" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3806,7 +3792,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4155,19 +4141,53 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="0" t="inlineStr">
         <is>
           <t>949vogeu</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月18日 11_38_38.png</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" s="0" t="inlineStr">
         <is>
           <t>2026-01-18 11:40:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="inlineStr">
+        <is>
+          <t>ghlktp23</t>
+        </is>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月20日 15_06_45.png</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>2026-01-20 15:08:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>ggu21lkq</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月20日 15_06_45.png</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2026-01-20 15:40:34</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-20 16:10:30
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A476"/>
+  <dimension ref="A1:A475"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -459,3323 +459,3316 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>j0writd2</t>
+          <t>vcjhum2r</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>vcjhum2r</t>
+          <t>fuxp1un3</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>fuxp1un3</t>
+          <t>dmy3qb36</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>dmy3qb36</t>
+          <t>3cs680lw</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>3cs680lw</t>
+          <t>3l5ikk8t</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>3l5ikk8t</t>
+          <t>8fcbyk1m</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>8fcbyk1m</t>
+          <t>y1puz53f</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>y1puz53f</t>
+          <t>f7m05b4u</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>f7m05b4u</t>
+          <t>axri1ag2</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>axri1ag2</t>
+          <t>n6s5h4v9</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>n6s5h4v9</t>
+          <t>lpv0bvsw</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>lpv0bvsw</t>
+          <t>p2ysb4km</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>p2ysb4km</t>
+          <t>0rh82tbc</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>r88cbjqo</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="474">
       <c r="A474" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="475">
       <c r="A475" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="476">
-      <c r="A476" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3792,7 +3785,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4175,19 +4168,36 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="0" t="inlineStr">
         <is>
           <t>ggu21lkq</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B23" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月20日 15_06_45.png</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C23" s="0" t="inlineStr">
         <is>
           <t>2026-01-20 15:40:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>j0writd2</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月20日 16_09_08.png</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2026-01-20 16:10:24</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-21 14:15:37
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A475"/>
+  <dimension ref="A1:A474"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -459,3316 +459,3309 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>vcjhum2r</t>
+          <t>fuxp1un3</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>fuxp1un3</t>
+          <t>dmy3qb36</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>dmy3qb36</t>
+          <t>3cs680lw</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>3cs680lw</t>
+          <t>3l5ikk8t</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>3l5ikk8t</t>
+          <t>8fcbyk1m</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>8fcbyk1m</t>
+          <t>y1puz53f</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>y1puz53f</t>
+          <t>f7m05b4u</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>f7m05b4u</t>
+          <t>axri1ag2</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>axri1ag2</t>
+          <t>n6s5h4v9</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>n6s5h4v9</t>
+          <t>lpv0bvsw</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>lpv0bvsw</t>
+          <t>p2ysb4km</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>p2ysb4km</t>
+          <t>0rh82tbc</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>r88cbjqo</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="474">
       <c r="A474" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="475">
-      <c r="A475" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3785,7 +3778,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4185,19 +4178,36 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="0" t="inlineStr">
         <is>
           <t>j0writd2</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月20日 16_09_08.png</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C24" s="0" t="inlineStr">
         <is>
           <t>2026-01-20 16:10:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>vcjhum2r</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 14_13_20.png</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2026-01-21 14:15:31</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-21 15:26:17
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A474"/>
+  <dimension ref="A1:A473"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -459,3309 +459,3302 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>fuxp1un3</t>
+          <t>dmy3qb36</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>dmy3qb36</t>
+          <t>3cs680lw</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>3cs680lw</t>
+          <t>3l5ikk8t</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>3l5ikk8t</t>
+          <t>8fcbyk1m</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>8fcbyk1m</t>
+          <t>y1puz53f</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>y1puz53f</t>
+          <t>f7m05b4u</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>f7m05b4u</t>
+          <t>axri1ag2</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>axri1ag2</t>
+          <t>n6s5h4v9</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>n6s5h4v9</t>
+          <t>lpv0bvsw</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>lpv0bvsw</t>
+          <t>p2ysb4km</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>p2ysb4km</t>
+          <t>0rh82tbc</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>r88cbjqo</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="474">
-      <c r="A474" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3778,7 +3771,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4195,19 +4188,36 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="0" t="inlineStr">
         <is>
           <t>vcjhum2r</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月21日 14_13_20.png</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C25" s="0" t="inlineStr">
         <is>
           <t>2026-01-21 14:15:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>fuxp1un3</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 15_24_19.png</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2026-01-21 15:26:11</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-21 15:31:25
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A473"/>
+  <dimension ref="A1:A472"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -459,3302 +459,3295 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>dmy3qb36</t>
+          <t>3cs680lw</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>3cs680lw</t>
+          <t>3l5ikk8t</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>3l5ikk8t</t>
+          <t>8fcbyk1m</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>8fcbyk1m</t>
+          <t>y1puz53f</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>y1puz53f</t>
+          <t>f7m05b4u</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>f7m05b4u</t>
+          <t>axri1ag2</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>axri1ag2</t>
+          <t>n6s5h4v9</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>n6s5h4v9</t>
+          <t>lpv0bvsw</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>lpv0bvsw</t>
+          <t>p2ysb4km</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>p2ysb4km</t>
+          <t>0rh82tbc</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>r88cbjqo</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="473">
-      <c r="A473" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3771,7 +3764,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4205,19 +4198,36 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="0" t="inlineStr">
         <is>
           <t>fuxp1un3</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月21日 15_24_19.png</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C26" s="0" t="inlineStr">
         <is>
           <t>2026-01-21 15:26:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>dmy3qb36</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 15_24_30.png</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2026-01-21 15:31:20</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-21 15:35:00
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A472"/>
+  <dimension ref="A1:A471"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -459,3295 +459,3288 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>3cs680lw</t>
+          <t>3l5ikk8t</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>3l5ikk8t</t>
+          <t>8fcbyk1m</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>8fcbyk1m</t>
+          <t>y1puz53f</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>y1puz53f</t>
+          <t>f7m05b4u</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>f7m05b4u</t>
+          <t>axri1ag2</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>axri1ag2</t>
+          <t>n6s5h4v9</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>n6s5h4v9</t>
+          <t>lpv0bvsw</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>lpv0bvsw</t>
+          <t>p2ysb4km</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>p2ysb4km</t>
+          <t>0rh82tbc</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>r88cbjqo</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="472">
-      <c r="A472" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3764,7 +3757,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4215,19 +4208,36 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="0" t="inlineStr">
         <is>
           <t>dmy3qb36</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B27" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月21日 15_24_30.png</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C27" s="0" t="inlineStr">
         <is>
           <t>2026-01-21 15:31:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>3cs680lw</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 15_24_34.png</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2026-01-21 15:34:54</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-21 15:38:01
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A471"/>
+  <dimension ref="A1:A470"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -459,3288 +459,3281 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>3l5ikk8t</t>
+          <t>8fcbyk1m</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>8fcbyk1m</t>
+          <t>y1puz53f</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>y1puz53f</t>
+          <t>f7m05b4u</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>f7m05b4u</t>
+          <t>axri1ag2</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>axri1ag2</t>
+          <t>n6s5h4v9</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>n6s5h4v9</t>
+          <t>lpv0bvsw</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>lpv0bvsw</t>
+          <t>p2ysb4km</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>p2ysb4km</t>
+          <t>0rh82tbc</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>r88cbjqo</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="471">
-      <c r="A471" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3757,7 +3750,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4225,19 +4218,36 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="0" t="inlineStr">
         <is>
           <t>3cs680lw</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月21日 15_24_34.png</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C28" s="0" t="inlineStr">
         <is>
           <t>2026-01-21 15:34:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>3l5ikk8t</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 15_24_40.png</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2026-01-21 15:37:55</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-21 15:48:30
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A470"/>
+  <dimension ref="A1:A468"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -459,3281 +459,3267 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>8fcbyk1m</t>
+          <t>f7m05b4u</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>y1puz53f</t>
+          <t>axri1ag2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>f7m05b4u</t>
+          <t>n6s5h4v9</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>axri1ag2</t>
+          <t>lpv0bvsw</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>n6s5h4v9</t>
+          <t>p2ysb4km</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>lpv0bvsw</t>
+          <t>0rh82tbc</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>p2ysb4km</t>
+          <t>r88cbjqo</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" s="0" t="inlineStr">
-        <is>
-          <t>c47md6bk</t>
-        </is>
-      </c>
-    </row>
-    <row r="469">
-      <c r="A469" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="470">
-      <c r="A470" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3750,7 +3736,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4235,19 +4221,53 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" s="0" t="inlineStr">
         <is>
           <t>3l5ikk8t</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B29" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月21日 15_24_40.png</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C29" s="0" t="inlineStr">
         <is>
           <t>2026-01-21 15:37:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>8fcbyk1m</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 15_47_37.png</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2026-01-21 15:48:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>y1puz53f</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 15_47_41.png</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2026-01-21 15:48:23</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-21 16:18:40
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A468"/>
+  <dimension ref="A1:A465"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -459,3267 +459,3246 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>f7m05b4u</t>
+          <t>lpv0bvsw</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>axri1ag2</t>
+          <t>p2ysb4km</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>n6s5h4v9</t>
+          <t>0rh82tbc</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>lpv0bvsw</t>
+          <t>r88cbjqo</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>p2ysb4km</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" s="0" t="inlineStr">
-        <is>
-          <t>bcj4kot7</t>
-        </is>
-      </c>
-    </row>
-    <row r="466">
-      <c r="A466" s="0" t="inlineStr">
-        <is>
-          <t>c47md6bk</t>
-        </is>
-      </c>
-    </row>
-    <row r="467">
-      <c r="A467" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="468">
-      <c r="A468" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3736,7 +3715,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4238,36 +4217,87 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="0" t="inlineStr">
         <is>
           <t>8fcbyk1m</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B30" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月21日 15_47_37.png</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C30" s="0" t="inlineStr">
         <is>
           <t>2026-01-21 15:48:23</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" s="0" t="inlineStr">
         <is>
           <t>y1puz53f</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B31" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月21日 15_47_41.png</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C31" s="0" t="inlineStr">
         <is>
           <t>2026-01-21 15:48:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>f7m05b4u</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 16_16_35.png</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2026-01-21 16:18:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>axri1ag2</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 16_16_46.png</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2026-01-21 16:18:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>n6s5h4v9</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 16_16_52.png</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2026-01-21 16:18:32</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-21 16:29:40
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A465"/>
+  <dimension ref="A1:A464"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -459,3246 +459,3239 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>lpv0bvsw</t>
+          <t>p2ysb4km</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>p2ysb4km</t>
+          <t>0rh82tbc</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>r88cbjqo</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="465">
-      <c r="A465" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3715,7 +3708,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4251,53 +4244,70 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" s="0" t="inlineStr">
         <is>
           <t>f7m05b4u</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B32" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月21日 16_16_35.png</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C32" s="0" t="inlineStr">
         <is>
           <t>2026-01-21 16:18:32</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="0" t="inlineStr">
         <is>
           <t>axri1ag2</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月21日 16_16_46.png</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C33" s="0" t="inlineStr">
         <is>
           <t>2026-01-21 16:18:32</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="0" t="inlineStr">
         <is>
           <t>n6s5h4v9</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月21日 16_16_52.png</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C34" s="0" t="inlineStr">
         <is>
           <t>2026-01-21 16:18:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>lpv0bvsw</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 16_28_28.png</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2026-01-21 16:29:33</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-21 16:40:47
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A464"/>
+  <dimension ref="A1:A463"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -459,3239 +459,3232 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>p2ysb4km</t>
+          <t>0rh82tbc</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>r88cbjqo</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="464">
-      <c r="A464" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3708,7 +3701,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4295,19 +4288,36 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35" s="0" t="inlineStr">
         <is>
           <t>lpv0bvsw</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B35" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月21日 16_28_28.png</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C35" s="0" t="inlineStr">
         <is>
           <t>2026-01-21 16:29:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>p2ysb4km</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 16_39_42.png</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2026-01-21 16:40:40</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-21 17:00:15
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A463"/>
+  <dimension ref="A1:A461"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -459,3232 +459,3218 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>0rh82tbc</t>
+          <t>qhnbcyxl</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>r88cbjqo</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" s="0" t="inlineStr">
-        <is>
-          <t>c47md6bk</t>
-        </is>
-      </c>
-    </row>
-    <row r="462">
-      <c r="A462" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="463">
-      <c r="A463" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3701,7 +3687,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4305,19 +4291,53 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="0" t="inlineStr">
         <is>
           <t>p2ysb4km</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B36" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月21日 16_39_42.png</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="C36" s="0" t="inlineStr">
         <is>
           <t>2026-01-21 16:40:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>0rh82tbc</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 16_55_57.png</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2026-01-21 17:00:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>r88cbjqo</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 16_58_50.png</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2026-01-21 17:00:07</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-21 17:13:01
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A461"/>
+  <dimension ref="A1:A460"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -459,3218 +459,3211 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>qhnbcyxl</t>
+          <t>zd9ff0d0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="461">
-      <c r="A461" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3687,7 +3680,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4308,36 +4301,53 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="0" t="inlineStr">
         <is>
           <t>0rh82tbc</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B37" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月21日 16_55_57.png</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C37" s="0" t="inlineStr">
         <is>
           <t>2026-01-21 17:00:07</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="0" t="inlineStr">
         <is>
           <t>r88cbjqo</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月21日 16_58_50.png</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="C38" s="0" t="inlineStr">
         <is>
           <t>2026-01-21 17:00:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>qhnbcyxl</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 17_12_08.png</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2026-01-21 17:12:54</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-21 17:22:18
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A460"/>
+  <dimension ref="A1:A459"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -459,3211 +459,3204 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>zd9ff0d0</t>
+          <t>gp69vuj4</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>cx8e8dvc</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="460">
-      <c r="A460" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3680,7 +3673,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4335,19 +4328,36 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" s="0" t="inlineStr">
         <is>
           <t>qhnbcyxl</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月21日 17_12_08.png</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="C39" s="0" t="inlineStr">
         <is>
           <t>2026-01-21 17:12:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>zd9ff0d0</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 17_21_37.png</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2026-01-21 17:22:11</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-21 20:58:22
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A459"/>
+  <dimension ref="A1:A457"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -459,3204 +459,3190 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>gp69vuj4</t>
+          <t>58jp6ymz</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>cx8e8dvc</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" s="0" t="inlineStr">
-        <is>
-          <t>c47md6bk</t>
-        </is>
-      </c>
-    </row>
-    <row r="458">
-      <c r="A458" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="459">
-      <c r="A459" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3673,7 +3659,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4345,19 +4331,53 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40" s="0" t="inlineStr">
         <is>
           <t>zd9ff0d0</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B40" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月21日 17_21_37.png</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C40" s="0" t="inlineStr">
         <is>
           <t>2026-01-21 17:22:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>gp69vuj4</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 20_56_59.png</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2026-01-21 20:58:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>cx8e8dvc</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 20_57_06.png</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2026-01-21 20:58:13</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-21 21:23:28
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A457"/>
+  <dimension ref="A1:A456"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -459,3190 +459,3183 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>58jp6ymz</t>
+          <t>2olgyqdi</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="457">
-      <c r="A457" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3659,7 +3652,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4348,36 +4341,53 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="0" t="inlineStr">
         <is>
           <t>gp69vuj4</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月21日 20_56_59.png</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C41" s="0" t="inlineStr">
         <is>
           <t>2026-01-21 20:58:13</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42" s="0" t="inlineStr">
         <is>
           <t>cx8e8dvc</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月21日 20_57_06.png</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C42" s="0" t="inlineStr">
         <is>
           <t>2026-01-21 20:58:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>58jp6ymz</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 21_22_39.png</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2026-01-21 21:23:20</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-21 21:37:53
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A456"/>
+  <dimension ref="A1:A455"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -459,3183 +459,3176 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>2olgyqdi</t>
+          <t>juub901g</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>lhgm2soo</t>
+          <t>l8t7smhu</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>l8t7smhu</t>
+          <t>fx1bziqe</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>fx1bziqe</t>
+          <t>zif77iv1</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>zif77iv1</t>
+          <t>r4d1daky</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>r4d1daky</t>
+          <t>o4qxde4m</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>o4qxde4m</t>
+          <t>bmcupdlx</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>bmcupdlx</t>
+          <t>oc482jbv</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>oc482jbv</t>
+          <t>46fxevkg</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>46fxevkg</t>
+          <t>e8fgl9fq</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>e8fgl9fq</t>
+          <t>cblqjbgr</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>cblqjbgr</t>
+          <t>qggw0cp2</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>qggw0cp2</t>
+          <t>7hfdc8dg</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>7hfdc8dg</t>
+          <t>c4ntzq0a</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>c4ntzq0a</t>
+          <t>l75c0x9d</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>l75c0x9d</t>
+          <t>nlyufgl6</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>nlyufgl6</t>
+          <t>7fzrrogi</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>7fzrrogi</t>
+          <t>xfe7itbq</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>xfe7itbq</t>
+          <t>jgcqf8lg</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>jgcqf8lg</t>
+          <t>y5wii1w8</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>y5wii1w8</t>
+          <t>e81r4mz5</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>e81r4mz5</t>
+          <t>l2s76dky</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>l2s76dky</t>
+          <t>2fov6r55</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>2fov6r55</t>
+          <t>nntzd9j8</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>nntzd9j8</t>
+          <t>isihw1tq</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>isihw1tq</t>
+          <t>8grklyk9</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>8grklyk9</t>
+          <t>oj3gh09e</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>oj3gh09e</t>
+          <t>0lt3jokj</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>0lt3jokj</t>
+          <t>b2kdy3t0</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>b2kdy3t0</t>
+          <t>wsaq3fs9</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>wsaq3fs9</t>
+          <t>yfl47xe9</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>yfl47xe9</t>
+          <t>05gjfzc0</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>05gjfzc0</t>
+          <t>q0uzcuzs</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>q0uzcuzs</t>
+          <t>rmm202kz</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>rmm202kz</t>
+          <t>iuprctsr</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>iuprctsr</t>
+          <t>lksu30tj</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>lksu30tj</t>
+          <t>tjuzz3gf</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>tjuzz3gf</t>
+          <t>0m30lkps</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>0m30lkps</t>
+          <t>8c21x355</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>8c21x355</t>
+          <t>bbygphk5</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>bbygphk5</t>
+          <t>1upjcwkw</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>1upjcwkw</t>
+          <t>1x43k23b</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>1x43k23b</t>
+          <t>f83i87w1</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>f83i87w1</t>
+          <t>ptvv9iuk</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>ptvv9iuk</t>
+          <t>18es3ste</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>18es3ste</t>
+          <t>krdaoi7n</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>krdaoi7n</t>
+          <t>4lch9pv6</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>4lch9pv6</t>
+          <t>5xgwxu47</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>5xgwxu47</t>
+          <t>pmehchex</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>pmehchex</t>
+          <t>r3t9t9qy</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>r3t9t9qy</t>
+          <t>xat323u4</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>xat323u4</t>
+          <t>sq4o3ivp</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>sq4o3ivp</t>
+          <t>prgbcl6n</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>prgbcl6n</t>
+          <t>kjgrabtz</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>kjgrabtz</t>
+          <t>mdjf24ko</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>mdjf24ko</t>
+          <t>anx40o66</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>anx40o66</t>
+          <t>4bijv6x9</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>4bijv6x9</t>
+          <t>swavpbzw</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>swavpbzw</t>
+          <t>080yifv2</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>080yifv2</t>
+          <t>6b85mmdr</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>6b85mmdr</t>
+          <t>po303w2k</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>po303w2k</t>
+          <t>bdcfqsng</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>bdcfqsng</t>
+          <t>clsy2k96</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>clsy2k96</t>
+          <t>u9wmlxht</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>u9wmlxht</t>
+          <t>h8riph3v</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>h8riph3v</t>
+          <t>fetd9t50</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>fetd9t50</t>
+          <t>7uw97ilc</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>7uw97ilc</t>
+          <t>ncg3x4dy</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>ncg3x4dy</t>
+          <t>s027q4u2</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>s027q4u2</t>
+          <t>bdgi96cy</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>bdgi96cy</t>
+          <t>cvueuw3r</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>cvueuw3r</t>
+          <t>e88ypiw4</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>e88ypiw4</t>
+          <t>vzi6yv18</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>vzi6yv18</t>
+          <t>3x4r8lbn</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>3x4r8lbn</t>
+          <t>0yiik65n</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>0yiik65n</t>
+          <t>wci8ag73</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>wci8ag73</t>
+          <t>rcha0kp5</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>rcha0kp5</t>
+          <t>500bec6m</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>500bec6m</t>
+          <t>wlv8kk2s</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>wlv8kk2s</t>
+          <t>01pf3i8r</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>01pf3i8r</t>
+          <t>t7hu6g7r</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>t7hu6g7r</t>
+          <t>065a0j4z</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>065a0j4z</t>
+          <t>83i4jgz8</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>83i4jgz8</t>
+          <t>xk6udito</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>xk6udito</t>
+          <t>20az5gci</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>20az5gci</t>
+          <t>ugvc2bkm</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>ugvc2bkm</t>
+          <t>nn93zcrh</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>nn93zcrh</t>
+          <t>yudxm1j7</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>yudxm1j7</t>
+          <t>rzdsrdb8</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>rzdsrdb8</t>
+          <t>wy8xgv6r</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>wy8xgv6r</t>
+          <t>bmm34y52</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>bmm34y52</t>
+          <t>w9621fg2</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>w9621fg2</t>
+          <t>va55amr2</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>va55amr2</t>
+          <t>ygd1dg0f</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>ygd1dg0f</t>
+          <t>udlkxats</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>udlkxats</t>
+          <t>g0lr79fj</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>g0lr79fj</t>
+          <t>w623sqk8</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>w623sqk8</t>
+          <t>d67h4x1i</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
-          <t>d67h4x1i</t>
+          <t>bm1841zs</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="inlineStr">
         <is>
-          <t>bm1841zs</t>
+          <t>mlo2lq8y</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="inlineStr">
         <is>
-          <t>mlo2lq8y</t>
+          <t>pw729iqj</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="inlineStr">
         <is>
-          <t>pw729iqj</t>
+          <t>uqdutnz7</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="inlineStr">
         <is>
-          <t>uqdutnz7</t>
+          <t>0z601p9z</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="inlineStr">
         <is>
-          <t>0z601p9z</t>
+          <t>56he7jjq</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="inlineStr">
         <is>
-          <t>56he7jjq</t>
+          <t>al6nomjg</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="inlineStr">
         <is>
-          <t>al6nomjg</t>
+          <t>d9jjvbaf</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="inlineStr">
         <is>
-          <t>d9jjvbaf</t>
+          <t>k2p4wfwz</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="inlineStr">
         <is>
-          <t>k2p4wfwz</t>
+          <t>6xjdh6w9</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="inlineStr">
         <is>
-          <t>6xjdh6w9</t>
+          <t>bhqq60df</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="inlineStr">
         <is>
-          <t>bhqq60df</t>
+          <t>vwrh51h2</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="inlineStr">
         <is>
-          <t>vwrh51h2</t>
+          <t>z0s3ab2o</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="inlineStr">
         <is>
-          <t>z0s3ab2o</t>
+          <t>n6legr5r</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="inlineStr">
         <is>
-          <t>n6legr5r</t>
+          <t>56j5g1jb</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="inlineStr">
         <is>
-          <t>56j5g1jb</t>
+          <t>bv58wjgu</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="inlineStr">
         <is>
-          <t>bv58wjgu</t>
+          <t>45grx220</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="inlineStr">
         <is>
-          <t>45grx220</t>
+          <t>5f53psep</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="inlineStr">
         <is>
-          <t>5f53psep</t>
+          <t>12p69nkq</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="inlineStr">
         <is>
-          <t>12p69nkq</t>
+          <t>xbox6gfi</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="inlineStr">
         <is>
-          <t>xbox6gfi</t>
+          <t>ocvvc4de</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="inlineStr">
         <is>
-          <t>ocvvc4de</t>
+          <t>bhoctcea</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="inlineStr">
         <is>
-          <t>bhoctcea</t>
+          <t>dq0n63xv</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="inlineStr">
         <is>
-          <t>dq0n63xv</t>
+          <t>xgyqhcrq</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="inlineStr">
         <is>
-          <t>xgyqhcrq</t>
+          <t>61ms931v</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="inlineStr">
         <is>
-          <t>61ms931v</t>
+          <t>cmd3a7uw</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="inlineStr">
         <is>
-          <t>cmd3a7uw</t>
+          <t>mle5icfw</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="inlineStr">
         <is>
-          <t>mle5icfw</t>
+          <t>i1jexett</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="inlineStr">
         <is>
-          <t>i1jexett</t>
+          <t>rkw2kjkv</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="inlineStr">
         <is>
-          <t>rkw2kjkv</t>
+          <t>0hi5kzz6</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="inlineStr">
         <is>
-          <t>0hi5kzz6</t>
+          <t>fb9tyqu8</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="inlineStr">
         <is>
-          <t>fb9tyqu8</t>
+          <t>cgje8ifp</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="inlineStr">
         <is>
-          <t>cgje8ifp</t>
+          <t>ds5x0s8e</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="inlineStr">
         <is>
-          <t>ds5x0s8e</t>
+          <t>se137g25</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="inlineStr">
         <is>
-          <t>se137g25</t>
+          <t>6hpd3btz</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="inlineStr">
         <is>
-          <t>6hpd3btz</t>
+          <t>w425hm0q</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="inlineStr">
         <is>
-          <t>w425hm0q</t>
+          <t>0yox2wxe</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="inlineStr">
         <is>
-          <t>0yox2wxe</t>
+          <t>61x5anay</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="inlineStr">
         <is>
-          <t>61x5anay</t>
+          <t>mk4py2gt</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="inlineStr">
         <is>
-          <t>mk4py2gt</t>
+          <t>ektoc356</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="inlineStr">
         <is>
-          <t>ektoc356</t>
+          <t>5z53uy6p</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="inlineStr">
         <is>
-          <t>5z53uy6p</t>
+          <t>sv5oxg0p</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="inlineStr">
         <is>
-          <t>sv5oxg0p</t>
+          <t>l2lm75bj</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="inlineStr">
         <is>
-          <t>l2lm75bj</t>
+          <t>u0cacv5y</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="inlineStr">
         <is>
-          <t>u0cacv5y</t>
+          <t>fkebpufq</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="inlineStr">
         <is>
-          <t>fkebpufq</t>
+          <t>8o3svusd</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="inlineStr">
         <is>
-          <t>8o3svusd</t>
+          <t>471m20yn</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="inlineStr">
         <is>
-          <t>471m20yn</t>
+          <t>g4mcalpz</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="inlineStr">
         <is>
-          <t>g4mcalpz</t>
+          <t>8v9dh1ti</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="inlineStr">
         <is>
-          <t>8v9dh1ti</t>
+          <t>u1w88uvf</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="inlineStr">
         <is>
-          <t>u1w88uvf</t>
+          <t>tkpbudsx</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="inlineStr">
         <is>
-          <t>tkpbudsx</t>
+          <t>6i48iawv</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="inlineStr">
         <is>
-          <t>6i48iawv</t>
+          <t>b6uzhvlc</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="inlineStr">
         <is>
-          <t>b6uzhvlc</t>
+          <t>xi04xomj</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="inlineStr">
         <is>
-          <t>xi04xomj</t>
+          <t>xyg886f4</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="inlineStr">
         <is>
-          <t>xyg886f4</t>
+          <t>44k2jpui</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="inlineStr">
         <is>
-          <t>44k2jpui</t>
+          <t>5qsu63x0</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="inlineStr">
         <is>
-          <t>5qsu63x0</t>
+          <t>7dwdg8kg</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="inlineStr">
         <is>
-          <t>7dwdg8kg</t>
+          <t>misl3skd</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="inlineStr">
         <is>
-          <t>misl3skd</t>
+          <t>spizy6dx</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="inlineStr">
         <is>
-          <t>spizy6dx</t>
+          <t>c3oxgeyn</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="inlineStr">
         <is>
-          <t>c3oxgeyn</t>
+          <t>8n7fzrcl</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="inlineStr">
         <is>
-          <t>8n7fzrcl</t>
+          <t>bvzvrdn9</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="inlineStr">
         <is>
-          <t>bvzvrdn9</t>
+          <t>xv1lc2bb</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="inlineStr">
         <is>
-          <t>xv1lc2bb</t>
+          <t>wd98y0gy</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="inlineStr">
         <is>
-          <t>wd98y0gy</t>
+          <t>96jy9axa</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="inlineStr">
         <is>
-          <t>96jy9axa</t>
+          <t>8cuikipm</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="inlineStr">
         <is>
-          <t>8cuikipm</t>
+          <t>pk65s8cb</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="inlineStr">
         <is>
-          <t>pk65s8cb</t>
+          <t>p4lwr66r</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="inlineStr">
         <is>
-          <t>p4lwr66r</t>
+          <t>q12hhpn0</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="inlineStr">
         <is>
-          <t>q12hhpn0</t>
+          <t>7hqd6rvw</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="inlineStr">
         <is>
-          <t>7hqd6rvw</t>
+          <t>htvshx9w</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="inlineStr">
         <is>
-          <t>htvshx9w</t>
+          <t>gdqa4lpy</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="inlineStr">
         <is>
-          <t>gdqa4lpy</t>
+          <t>vyjd40c1</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="inlineStr">
         <is>
-          <t>vyjd40c1</t>
+          <t>7uydvumo</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="inlineStr">
         <is>
-          <t>7uydvumo</t>
+          <t>arrfzncu</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="inlineStr">
         <is>
-          <t>arrfzncu</t>
+          <t>dvrym24p</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="inlineStr">
         <is>
-          <t>dvrym24p</t>
+          <t>pjwje7vu</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="inlineStr">
         <is>
-          <t>pjwje7vu</t>
+          <t>6zheeauc</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="inlineStr">
         <is>
-          <t>6zheeauc</t>
+          <t>1rq140k5</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="inlineStr">
         <is>
-          <t>1rq140k5</t>
+          <t>cn0y0fpw</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="inlineStr">
         <is>
-          <t>cn0y0fpw</t>
+          <t>7syf56sf</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="inlineStr">
         <is>
-          <t>7syf56sf</t>
+          <t>71dnxhy9</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="inlineStr">
         <is>
-          <t>71dnxhy9</t>
+          <t>nabpk9ae</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="inlineStr">
         <is>
-          <t>nabpk9ae</t>
+          <t>izib4vye</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="inlineStr">
         <is>
-          <t>izib4vye</t>
+          <t>6w4gzpsj</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="inlineStr">
         <is>
-          <t>6w4gzpsj</t>
+          <t>q7ilytx4</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="inlineStr">
         <is>
-          <t>q7ilytx4</t>
+          <t>tn5m69zv</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="inlineStr">
         <is>
-          <t>tn5m69zv</t>
+          <t>hxlzj4xe</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="inlineStr">
         <is>
-          <t>hxlzj4xe</t>
+          <t>tn0rvikr</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="inlineStr">
         <is>
-          <t>tn0rvikr</t>
+          <t>gcifrp1f</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="inlineStr">
         <is>
-          <t>gcifrp1f</t>
+          <t>fswpebtf</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="inlineStr">
         <is>
-          <t>fswpebtf</t>
+          <t>399gdc11</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="inlineStr">
         <is>
-          <t>399gdc11</t>
+          <t>ugmuiba4</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="inlineStr">
         <is>
-          <t>ugmuiba4</t>
+          <t>fvk9gam2</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="inlineStr">
         <is>
-          <t>fvk9gam2</t>
+          <t>au0h72t0</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="inlineStr">
         <is>
-          <t>au0h72t0</t>
+          <t>4wjlxqmm</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="inlineStr">
         <is>
-          <t>4wjlxqmm</t>
+          <t>itvf2ud5</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="inlineStr">
         <is>
-          <t>itvf2ud5</t>
+          <t>yikrbdal</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="inlineStr">
         <is>
-          <t>yikrbdal</t>
+          <t>vwzt6ime</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="inlineStr">
         <is>
-          <t>vwzt6ime</t>
+          <t>fgtpane9</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="inlineStr">
         <is>
-          <t>fgtpane9</t>
+          <t>rh11i1yv</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="inlineStr">
         <is>
-          <t>rh11i1yv</t>
+          <t>zmpyphkc</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="inlineStr">
         <is>
-          <t>zmpyphkc</t>
+          <t>v00gatq2</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="inlineStr">
         <is>
-          <t>v00gatq2</t>
+          <t>ejrvaoru</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="inlineStr">
         <is>
-          <t>ejrvaoru</t>
+          <t>hhzurczn</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="inlineStr">
         <is>
-          <t>hhzurczn</t>
+          <t>qln5un5w</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="inlineStr">
         <is>
-          <t>qln5un5w</t>
+          <t>iolq5mnt</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="inlineStr">
         <is>
-          <t>iolq5mnt</t>
+          <t>yl0n41ra</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="inlineStr">
         <is>
-          <t>yl0n41ra</t>
+          <t>wx2d6jtk</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="inlineStr">
         <is>
-          <t>wx2d6jtk</t>
+          <t>3k50dezu</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="inlineStr">
         <is>
-          <t>3k50dezu</t>
+          <t>pa5h6r35</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="inlineStr">
         <is>
-          <t>pa5h6r35</t>
+          <t>z8jh9a8k</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="inlineStr">
         <is>
-          <t>z8jh9a8k</t>
+          <t>5ms931fj</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="inlineStr">
         <is>
-          <t>5ms931fj</t>
+          <t>t62s84o4</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="inlineStr">
         <is>
-          <t>t62s84o4</t>
+          <t>2725haxj</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="inlineStr">
         <is>
-          <t>2725haxj</t>
+          <t>8s66niwi</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="inlineStr">
         <is>
-          <t>8s66niwi</t>
+          <t>bz58komx</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="inlineStr">
         <is>
-          <t>bz58komx</t>
+          <t>96syts4o</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="inlineStr">
         <is>
-          <t>96syts4o</t>
+          <t>7lbeo8bb</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="inlineStr">
         <is>
-          <t>7lbeo8bb</t>
+          <t>0c8au105</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="inlineStr">
         <is>
-          <t>0c8au105</t>
+          <t>vr8r9y5c</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="inlineStr">
         <is>
-          <t>vr8r9y5c</t>
+          <t>wh8hja6z</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="inlineStr">
         <is>
-          <t>wh8hja6z</t>
+          <t>x2b6yrpj</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="inlineStr">
         <is>
-          <t>x2b6yrpj</t>
+          <t>qomowuz6</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="inlineStr">
         <is>
-          <t>qomowuz6</t>
+          <t>nsa4f9vm</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="inlineStr">
         <is>
-          <t>nsa4f9vm</t>
+          <t>ozdthkmx</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="inlineStr">
         <is>
-          <t>ozdthkmx</t>
+          <t>3a2b0b1k</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="inlineStr">
         <is>
-          <t>3a2b0b1k</t>
+          <t>55d16gxr</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="inlineStr">
         <is>
-          <t>55d16gxr</t>
+          <t>e8z0blzr</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="inlineStr">
         <is>
-          <t>e8z0blzr</t>
+          <t>91h21hc7</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="inlineStr">
         <is>
-          <t>91h21hc7</t>
+          <t>jd96333l</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="inlineStr">
         <is>
-          <t>jd96333l</t>
+          <t>c8cdo3to</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="inlineStr">
         <is>
-          <t>c8cdo3to</t>
+          <t>57vf22yl</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="inlineStr">
         <is>
-          <t>57vf22yl</t>
+          <t>inuurtz9</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="inlineStr">
         <is>
-          <t>inuurtz9</t>
+          <t>b89dfmdo</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="inlineStr">
         <is>
-          <t>b89dfmdo</t>
+          <t>thoyx4cb</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="inlineStr">
         <is>
-          <t>thoyx4cb</t>
+          <t>cfut1re7</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="inlineStr">
         <is>
-          <t>cfut1re7</t>
+          <t>336rjmr7</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="inlineStr">
         <is>
-          <t>336rjmr7</t>
+          <t>0ppbbodb</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="inlineStr">
         <is>
-          <t>0ppbbodb</t>
+          <t>7cajfvi0</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="inlineStr">
         <is>
-          <t>7cajfvi0</t>
+          <t>panua1c2</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="inlineStr">
         <is>
-          <t>panua1c2</t>
+          <t>u2e6dxsi</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="inlineStr">
         <is>
-          <t>u2e6dxsi</t>
+          <t>r5jous05</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="inlineStr">
         <is>
-          <t>r5jous05</t>
+          <t>r5tqiey9</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="inlineStr">
         <is>
-          <t>r5tqiey9</t>
+          <t>acs4ofv8</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="inlineStr">
         <is>
-          <t>acs4ofv8</t>
+          <t>kne43ydl</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="inlineStr">
         <is>
-          <t>kne43ydl</t>
+          <t>u6gqbdnd</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="inlineStr">
         <is>
-          <t>u6gqbdnd</t>
+          <t>si4ti5qv</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="inlineStr">
         <is>
-          <t>si4ti5qv</t>
+          <t>hikr2p7n</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="inlineStr">
         <is>
-          <t>hikr2p7n</t>
+          <t>sjtg37c6</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="inlineStr">
         <is>
-          <t>sjtg37c6</t>
+          <t>jabjcn86</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="inlineStr">
         <is>
-          <t>jabjcn86</t>
+          <t>ha7gc51l</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="inlineStr">
         <is>
-          <t>ha7gc51l</t>
+          <t>qmji87hq</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="inlineStr">
         <is>
-          <t>qmji87hq</t>
+          <t>sdbc4x5n</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="inlineStr">
         <is>
-          <t>sdbc4x5n</t>
+          <t>3tep5l7z</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="inlineStr">
         <is>
-          <t>3tep5l7z</t>
+          <t>f776qp8a</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="inlineStr">
         <is>
-          <t>f776qp8a</t>
+          <t>a9nfp88y</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="inlineStr">
         <is>
-          <t>a9nfp88y</t>
+          <t>n0v0uh4f</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="inlineStr">
         <is>
-          <t>n0v0uh4f</t>
+          <t>hjordi3b</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="inlineStr">
         <is>
-          <t>hjordi3b</t>
+          <t>nn5c0nuf</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="inlineStr">
         <is>
-          <t>nn5c0nuf</t>
+          <t>ri8ihyzi</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="inlineStr">
         <is>
-          <t>ri8ihyzi</t>
+          <t>v7kf2u0v</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="inlineStr">
         <is>
-          <t>v7kf2u0v</t>
+          <t>9tthrsoa</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="inlineStr">
         <is>
-          <t>9tthrsoa</t>
+          <t>1m3wq5v9</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="inlineStr">
         <is>
-          <t>1m3wq5v9</t>
+          <t>zly73s0w</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="inlineStr">
         <is>
-          <t>zly73s0w</t>
+          <t>ffc0ksyr</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="inlineStr">
         <is>
-          <t>ffc0ksyr</t>
+          <t>vxf3dm0q</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="inlineStr">
         <is>
-          <t>vxf3dm0q</t>
+          <t>egbgz3eu</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="inlineStr">
         <is>
-          <t>egbgz3eu</t>
+          <t>hu6ry1j1</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="inlineStr">
         <is>
-          <t>hu6ry1j1</t>
+          <t>r38omu6y</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="inlineStr">
         <is>
-          <t>r38omu6y</t>
+          <t>myx5e7p8</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="inlineStr">
         <is>
-          <t>myx5e7p8</t>
+          <t>p20vyzcr</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="inlineStr">
         <is>
-          <t>p20vyzcr</t>
+          <t>wpucxfgx</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="inlineStr">
         <is>
-          <t>wpucxfgx</t>
+          <t>341ae00s</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="inlineStr">
         <is>
-          <t>341ae00s</t>
+          <t>8o49iagt</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="inlineStr">
         <is>
-          <t>8o49iagt</t>
+          <t>cx78vrhy</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="inlineStr">
         <is>
-          <t>cx78vrhy</t>
+          <t>7gpd7npb</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="inlineStr">
         <is>
-          <t>7gpd7npb</t>
+          <t>37m7n6lu</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="inlineStr">
         <is>
-          <t>37m7n6lu</t>
+          <t>ytoqheub</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="inlineStr">
         <is>
-          <t>ytoqheub</t>
+          <t>pqj15c3x</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="inlineStr">
         <is>
-          <t>pqj15c3x</t>
+          <t>nnx2fc52</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="inlineStr">
         <is>
-          <t>nnx2fc52</t>
+          <t>fu86nuzc</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="inlineStr">
         <is>
-          <t>fu86nuzc</t>
+          <t>g5p993al</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="inlineStr">
         <is>
-          <t>g5p993al</t>
+          <t>4igsxwtk</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="inlineStr">
         <is>
-          <t>4igsxwtk</t>
+          <t>2k65tpne</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="inlineStr">
         <is>
-          <t>2k65tpne</t>
+          <t>ohuo3364</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="inlineStr">
         <is>
-          <t>ohuo3364</t>
+          <t>ruo014or</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="inlineStr">
         <is>
-          <t>ruo014or</t>
+          <t>tg3glnce</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="inlineStr">
         <is>
-          <t>tg3glnce</t>
+          <t>gz27zz2h</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="inlineStr">
         <is>
-          <t>gz27zz2h</t>
+          <t>sq53n3mv</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="inlineStr">
         <is>
-          <t>sq53n3mv</t>
+          <t>dq4jaxu5</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="inlineStr">
         <is>
-          <t>dq4jaxu5</t>
+          <t>eidipki9</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="inlineStr">
         <is>
-          <t>eidipki9</t>
+          <t>syzletxk</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="inlineStr">
         <is>
-          <t>syzletxk</t>
+          <t>l9wtzu5m</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="inlineStr">
         <is>
-          <t>l9wtzu5m</t>
+          <t>sphem018</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="inlineStr">
         <is>
-          <t>sphem018</t>
+          <t>3don6chr</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="inlineStr">
         <is>
-          <t>3don6chr</t>
+          <t>d5astwnm</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="inlineStr">
         <is>
-          <t>d5astwnm</t>
+          <t>fiznp08b</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="inlineStr">
         <is>
-          <t>fiznp08b</t>
+          <t>wpwejt83</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="inlineStr">
         <is>
-          <t>wpwejt83</t>
+          <t>c9daevlg</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="inlineStr">
         <is>
-          <t>c9daevlg</t>
+          <t>wwr84ot4</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="inlineStr">
         <is>
-          <t>wwr84ot4</t>
+          <t>n58zlpqa</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="inlineStr">
         <is>
-          <t>n58zlpqa</t>
+          <t>0ed31ce7</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="inlineStr">
         <is>
-          <t>0ed31ce7</t>
+          <t>wpkahmqb</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="inlineStr">
         <is>
-          <t>wpkahmqb</t>
+          <t>7tykrz3e</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="inlineStr">
         <is>
-          <t>7tykrz3e</t>
+          <t>eafga75g</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="inlineStr">
         <is>
-          <t>eafga75g</t>
+          <t>sygdbaqi</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="inlineStr">
         <is>
-          <t>sygdbaqi</t>
+          <t>l6pebkmu</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="inlineStr">
         <is>
-          <t>l6pebkmu</t>
+          <t>uiw7mi8t</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="inlineStr">
         <is>
-          <t>uiw7mi8t</t>
+          <t>urh9w0pf</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="inlineStr">
         <is>
-          <t>urh9w0pf</t>
+          <t>nt9xdo0b</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="inlineStr">
         <is>
-          <t>nt9xdo0b</t>
+          <t>c1lntaw0</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="inlineStr">
         <is>
-          <t>c1lntaw0</t>
+          <t>yusgfy1y</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="inlineStr">
         <is>
-          <t>yusgfy1y</t>
+          <t>w2r20qg9</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="inlineStr">
         <is>
-          <t>w2r20qg9</t>
+          <t>vt71msfc</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="inlineStr">
         <is>
-          <t>vt71msfc</t>
+          <t>0y6mrn2m</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="inlineStr">
         <is>
-          <t>0y6mrn2m</t>
+          <t>oaqzbqkh</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="inlineStr">
         <is>
-          <t>oaqzbqkh</t>
+          <t>2ojh5tuk</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="inlineStr">
         <is>
-          <t>2ojh5tuk</t>
+          <t>yes9z8oh</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="inlineStr">
         <is>
-          <t>yes9z8oh</t>
+          <t>4up1m5dc</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="inlineStr">
         <is>
-          <t>4up1m5dc</t>
+          <t>a99hmzpf</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="inlineStr">
         <is>
-          <t>a99hmzpf</t>
+          <t>i2q4ysrd</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="inlineStr">
         <is>
-          <t>i2q4ysrd</t>
+          <t>vu34fi2t</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="inlineStr">
         <is>
-          <t>vu34fi2t</t>
+          <t>chc0akha</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="inlineStr">
         <is>
-          <t>chc0akha</t>
+          <t>ef75nbm5</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="inlineStr">
         <is>
-          <t>ef75nbm5</t>
+          <t>30rzzev7</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="inlineStr">
         <is>
-          <t>30rzzev7</t>
+          <t>i2yg73h2</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="inlineStr">
         <is>
-          <t>i2yg73h2</t>
+          <t>tysjapcw</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="inlineStr">
         <is>
-          <t>tysjapcw</t>
+          <t>7ast57js</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="inlineStr">
         <is>
-          <t>7ast57js</t>
+          <t>3g8suxhx</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="inlineStr">
         <is>
-          <t>3g8suxhx</t>
+          <t>rtxbdtn0</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="inlineStr">
         <is>
-          <t>rtxbdtn0</t>
+          <t>4fcptj2n</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="inlineStr">
         <is>
-          <t>4fcptj2n</t>
+          <t>xze7ye5z</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="inlineStr">
         <is>
-          <t>xze7ye5z</t>
+          <t>k57hftpu</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="inlineStr">
         <is>
-          <t>k57hftpu</t>
+          <t>lovperfz</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="inlineStr">
         <is>
-          <t>lovperfz</t>
+          <t>8717peki</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="inlineStr">
         <is>
-          <t>8717peki</t>
+          <t>lvjbftc3</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="0" t="inlineStr">
         <is>
-          <t>lvjbftc3</t>
+          <t>w6wkmz1p</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="0" t="inlineStr">
         <is>
-          <t>w6wkmz1p</t>
+          <t>rp23p95f</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="0" t="inlineStr">
         <is>
-          <t>rp23p95f</t>
+          <t>mbwrybja</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="0" t="inlineStr">
         <is>
-          <t>mbwrybja</t>
+          <t>rkn4zmxh</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="0" t="inlineStr">
         <is>
-          <t>rkn4zmxh</t>
+          <t>3rsl3bwp</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="0" t="inlineStr">
         <is>
-          <t>3rsl3bwp</t>
+          <t>1dsh3cyl</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="0" t="inlineStr">
         <is>
-          <t>1dsh3cyl</t>
+          <t>j68i7zgm</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="0" t="inlineStr">
         <is>
-          <t>j68i7zgm</t>
+          <t>wx2x70e3</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="0" t="inlineStr">
         <is>
-          <t>wx2x70e3</t>
+          <t>fopi9zhe</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="0" t="inlineStr">
         <is>
-          <t>fopi9zhe</t>
+          <t>1v9mtzwe</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="0" t="inlineStr">
         <is>
-          <t>1v9mtzwe</t>
+          <t>xf3rhd7t</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="0" t="inlineStr">
         <is>
-          <t>xf3rhd7t</t>
+          <t>c2295nkt</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="0" t="inlineStr">
         <is>
-          <t>c2295nkt</t>
+          <t>8vzr5hsl</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="0" t="inlineStr">
         <is>
-          <t>8vzr5hsl</t>
+          <t>8ig2vwru</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="0" t="inlineStr">
         <is>
-          <t>8ig2vwru</t>
+          <t>hgb688xy</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="0" t="inlineStr">
         <is>
-          <t>hgb688xy</t>
+          <t>19t54xnr</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="0" t="inlineStr">
         <is>
-          <t>19t54xnr</t>
+          <t>0xzdr5e7</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="0" t="inlineStr">
         <is>
-          <t>0xzdr5e7</t>
+          <t>aya7z42b</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="0" t="inlineStr">
         <is>
-          <t>aya7z42b</t>
+          <t>l2nwlokc</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="0" t="inlineStr">
         <is>
-          <t>l2nwlokc</t>
+          <t>wcn0f14m</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="0" t="inlineStr">
         <is>
-          <t>wcn0f14m</t>
+          <t>cukxbo4y</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="0" t="inlineStr">
         <is>
-          <t>cukxbo4y</t>
+          <t>c94ze19c</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="0" t="inlineStr">
         <is>
-          <t>c94ze19c</t>
+          <t>hg9656tr</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="0" t="inlineStr">
         <is>
-          <t>hg9656tr</t>
+          <t>e6lzp8ff</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="0" t="inlineStr">
         <is>
-          <t>e6lzp8ff</t>
+          <t>y7ceasgw</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="0" t="inlineStr">
         <is>
-          <t>y7ceasgw</t>
+          <t>7xqh0b3n</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="0" t="inlineStr">
         <is>
-          <t>7xqh0b3n</t>
+          <t>aywbjf79</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="0" t="inlineStr">
         <is>
-          <t>aywbjf79</t>
+          <t>oikatzhh</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="0" t="inlineStr">
         <is>
-          <t>oikatzhh</t>
+          <t>49zdakl1</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="0" t="inlineStr">
         <is>
-          <t>49zdakl1</t>
+          <t>j6v6oehf</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="0" t="inlineStr">
         <is>
-          <t>j6v6oehf</t>
+          <t>bv05pxfl</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="0" t="inlineStr">
         <is>
-          <t>bv05pxfl</t>
+          <t>icb9014m</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="0" t="inlineStr">
         <is>
-          <t>icb9014m</t>
+          <t>x71hzadt</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="0" t="inlineStr">
         <is>
-          <t>x71hzadt</t>
+          <t>z66nyx8a</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="0" t="inlineStr">
         <is>
-          <t>z66nyx8a</t>
+          <t>6rtbyl9n</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="0" t="inlineStr">
         <is>
-          <t>6rtbyl9n</t>
+          <t>l69u7cq9</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="0" t="inlineStr">
         <is>
-          <t>l69u7cq9</t>
+          <t>6ijo3rku</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="0" t="inlineStr">
         <is>
-          <t>6ijo3rku</t>
+          <t>g75gntpm</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="0" t="inlineStr">
         <is>
-          <t>g75gntpm</t>
+          <t>7oewonw7</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="0" t="inlineStr">
         <is>
-          <t>7oewonw7</t>
+          <t>wgwy1228</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="0" t="inlineStr">
         <is>
-          <t>wgwy1228</t>
+          <t>dcstvt9d</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="0" t="inlineStr">
         <is>
-          <t>dcstvt9d</t>
+          <t>z6w2yvgy</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="0" t="inlineStr">
         <is>
-          <t>z6w2yvgy</t>
+          <t>eme0z3s1</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="0" t="inlineStr">
         <is>
-          <t>eme0z3s1</t>
+          <t>wroijhyi</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="0" t="inlineStr">
         <is>
-          <t>wroijhyi</t>
+          <t>7b6ouc5n</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="0" t="inlineStr">
         <is>
-          <t>7b6ouc5n</t>
+          <t>vy4hrqud</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="0" t="inlineStr">
         <is>
-          <t>vy4hrqud</t>
+          <t>qp60bkdh</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="0" t="inlineStr">
         <is>
-          <t>qp60bkdh</t>
+          <t>jnlsbnbm</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="0" t="inlineStr">
         <is>
-          <t>jnlsbnbm</t>
+          <t>h938r2dg</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="0" t="inlineStr">
         <is>
-          <t>h938r2dg</t>
+          <t>gqpvtqlg</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="0" t="inlineStr">
         <is>
-          <t>gqpvtqlg</t>
+          <t>l090dgws</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="0" t="inlineStr">
         <is>
-          <t>l090dgws</t>
+          <t>ivc534ko</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="0" t="inlineStr">
         <is>
-          <t>ivc534ko</t>
+          <t>olxj4lpd</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="0" t="inlineStr">
         <is>
-          <t>olxj4lpd</t>
+          <t>480trr62</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="0" t="inlineStr">
         <is>
-          <t>480trr62</t>
+          <t>jht7ws2l</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="0" t="inlineStr">
         <is>
-          <t>jht7ws2l</t>
+          <t>cxxny6lb</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="0" t="inlineStr">
         <is>
-          <t>cxxny6lb</t>
+          <t>nqvsbunw</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="0" t="inlineStr">
         <is>
-          <t>nqvsbunw</t>
+          <t>m58vcmrq</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="0" t="inlineStr">
         <is>
-          <t>m58vcmrq</t>
+          <t>fkvndz1e</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="0" t="inlineStr">
         <is>
-          <t>fkvndz1e</t>
+          <t>2ryp8pdv</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="0" t="inlineStr">
         <is>
-          <t>2ryp8pdv</t>
+          <t>p6pdiftq</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="0" t="inlineStr">
         <is>
-          <t>p6pdiftq</t>
+          <t>usoqsqpd</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="0" t="inlineStr">
         <is>
-          <t>usoqsqpd</t>
+          <t>m15ggta1</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="0" t="inlineStr">
         <is>
-          <t>m15ggta1</t>
+          <t>midox0sh</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="0" t="inlineStr">
         <is>
-          <t>midox0sh</t>
+          <t>h5klasbv</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="0" t="inlineStr">
         <is>
-          <t>h5klasbv</t>
+          <t>6iwhgtlz</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="0" t="inlineStr">
         <is>
-          <t>6iwhgtlz</t>
+          <t>fzjn4mak</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="0" t="inlineStr">
         <is>
-          <t>fzjn4mak</t>
+          <t>4ckdv838</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="0" t="inlineStr">
         <is>
-          <t>4ckdv838</t>
+          <t>21wz9ew7</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="0" t="inlineStr">
         <is>
-          <t>21wz9ew7</t>
+          <t>6u4jmsfn</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="0" t="inlineStr">
         <is>
-          <t>6u4jmsfn</t>
+          <t>1bvc1uqc</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="0" t="inlineStr">
         <is>
-          <t>1bvc1uqc</t>
+          <t>gdwuju2b</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="0" t="inlineStr">
         <is>
-          <t>gdwuju2b</t>
+          <t>xjjta8wu</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="0" t="inlineStr">
         <is>
-          <t>xjjta8wu</t>
+          <t>kwkme77z</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="0" t="inlineStr">
         <is>
-          <t>kwkme77z</t>
+          <t>jn54e8jg</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="0" t="inlineStr">
         <is>
-          <t>jn54e8jg</t>
+          <t>ujez4vph</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="0" t="inlineStr">
         <is>
-          <t>ujez4vph</t>
+          <t>i7b2hipv</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="0" t="inlineStr">
         <is>
-          <t>i7b2hipv</t>
+          <t>118m8b7c</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="0" t="inlineStr">
         <is>
-          <t>118m8b7c</t>
+          <t>tlwa9cdc</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="0" t="inlineStr">
         <is>
-          <t>tlwa9cdc</t>
+          <t>mtrzkme4</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="0" t="inlineStr">
         <is>
-          <t>mtrzkme4</t>
+          <t>5i8q60rb</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" s="0" t="inlineStr">
         <is>
-          <t>5i8q60rb</t>
+          <t>bcj4kot7</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" s="0" t="inlineStr">
         <is>
-          <t>bcj4kot7</t>
+          <t>c47md6bk</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" s="0" t="inlineStr">
         <is>
-          <t>c47md6bk</t>
+          <t>oep6zrkl</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" s="0" t="inlineStr">
-        <is>
-          <t>oep6zrkl</t>
-        </is>
-      </c>
-    </row>
-    <row r="456">
-      <c r="A456" s="0" t="inlineStr">
         <is>
           <t>qvftx0of</t>
         </is>
@@ -3652,7 +3645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4375,19 +4368,36 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="A43" s="0" t="inlineStr">
         <is>
           <t>58jp6ymz</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B43" s="0" t="inlineStr">
         <is>
           <t>ChatGPT Image 2026年1月21日 21_22_39.png</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C43" s="0" t="inlineStr">
         <is>
           <t>2026-01-21 21:23:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2olgyqdi</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ChatGPT Image 2026年1月21日 21_36_51.png</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2026-01-21 21:37:45</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update works images 2026-01-22 15:56:06
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A455"/>
+  <dimension ref="A1:A454"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -459,3176 +459,3169 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>juub901g</t>
+          <t>eao5ane8</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>eao5ane8</t>
+          <t>rhe1j7fa</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>rhe1j7fa</t>
+          <t>omp3oay0</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>omp3oay0</t>
+          <t>w7jh25nq</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>w7jh25nq</t>
+          <t>nc0b4z5l</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>nc0b4z5l</t>
+          <t>65r5yqw0</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>65r5yqw0</t>
+          <t>it46z8y8</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>it46z8y8</t>
+          <t>zix3cm7k</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>zix3cm7k</t>
+          <t>rzjcqs4c</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>rzjcqs4c</t>
+          <t>zt252cs6</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>zt252cs6</t>
+          <t>8bve07yj</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>8bve07yj</t>
+          <t>jgk9ihfd</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>jgk9ihfd</t>
+          <t>3vqb9o6r</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>3vqb9o6r</t>
+          <t>4fjbj1hu</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>4fjbj1hu</t>
+          <t>mwhgtr34</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>mwhgtr34</t>
+          <t>fu7egmqg</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>fu7egmqg</t>
+          <t>q455aarn</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>q455aarn</t>
+          <t>xp5us0hq</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>xp5us0hq</t>
+          <t>lfrrqlph</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>lfrrqlph</t>
+          <t>54opnusx</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>54opnusx</t>
+          <t>d6a4w70z</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>d6a4w70z</t>
+          <t>cf2nuj5b</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>cf2nuj5b</t>
+          <t>v2i8st19</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>v2i8st19</t>
+          <t>cwvznz5t</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>cwvznz5t</t>
+          <t>nz6iz6q1</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>nz6iz6q1</t>
+          <t>utgci9pb</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>utgci9pb</t>
+          <t>ckwx7dtd</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>ckwx7dtd</t>
+          <t>wpx4tbqv</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>wpx4tbqv</t>
+          <t>0xrhz7td</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>0xrhz7td</t>
+          <t>ps5oiwgv</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>ps5oiwgv</t>
+          <t>07mg5zg3</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>07mg5zg3</t>
+          <t>ac2r5apc</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>ac2r5apc</t>
+          <t>lhgm2soo</t>
         </is>
       </c>
     </row>
     <row r="35">
